<commit_message>
feature analysis, results analysis, cleanup
</commit_message>
<xml_diff>
--- a/Feature Analysis/DT_analysis.xlsx
+++ b/Feature Analysis/DT_analysis.xlsx
@@ -8,20 +8,63 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/barberademol/Desktop/MLanalysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3BDB64AB-166E-CE4D-8BCE-BDE891850524}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{C0554CE0-9D84-5E46-B3EB-5A6FB1DD3410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="960" windowWidth="27160" windowHeight="16540" activeTab="1"/>
+    <workbookView xWindow="860" yWindow="460" windowWidth="27940" windowHeight="17540" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="DT_analysis" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="imported" sheetId="2" r:id="rId2"/>
+    <sheet name="abs" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">abs!$A$1:$D$1</definedName>
+    <definedName name="DT_analysis" localSheetId="1">imported!#REF!</definedName>
+    <definedName name="DT_analysis_1" localSheetId="2">abs!$A$1:$D$54</definedName>
+    <definedName name="DT_analysis_1" localSheetId="1">imported!$A$1:$D$54</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
+<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" name="DT_analysis1" type="6" refreshedVersion="7" background="1" saveData="1">
+    <textPr sourceFile="/Users/barberademol/Desktop/ML_12/DT_analysis.csv" decimal="," thousands="." comma="1">
+      <textFields count="4">
+        <textField/>
+        <textField/>
+        <textField type="text"/>
+        <textField type="text"/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="2" name="DT_analysis11" type="6" refreshedVersion="7" background="1" saveData="1">
+    <textPr sourceFile="/Users/barberademol/Desktop/ML_12/DT_analysis.csv" decimal="," thousands="." comma="1">
+      <textFields count="4">
+        <textField/>
+        <textField/>
+        <textField type="text"/>
+        <textField type="text"/>
+      </textFields>
+    </textPr>
+  </connection>
+</connections>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="57">
   <si>
     <t>,Principal Component Vector Number,class1,class2</t>
   </si>
@@ -183,12 +226,24 @@
   </si>
   <si>
     <t>52,53,0.0077457540362754805,-0.0077457540362754805</t>
+  </si>
+  <si>
+    <t>Principal Component Vector Number</t>
+  </si>
+  <si>
+    <t>class1</t>
+  </si>
+  <si>
+    <t>class2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="180" formatCode="0.000000000000000000"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -666,8 +721,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -724,6 +783,14 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DT_analysis_1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DT_analysis_1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1025,7 +1092,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A54"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -1306,12 +1375,1659 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="A1:D54"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>45</v>
+      </c>
+      <c r="B2">
+        <v>46</v>
+      </c>
+      <c r="C2" s="2">
+        <v>7.5521497601685304E-5</v>
+      </c>
+      <c r="D2" s="2">
+        <v>-7.5521497601685399E-5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>28</v>
+      </c>
+      <c r="B3">
+        <v>29</v>
+      </c>
+      <c r="C3" s="2">
+        <v>6.5715416017797106E-5</v>
+      </c>
+      <c r="D3" s="2">
+        <v>-6.5715416017797106E-5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>10</v>
+      </c>
+      <c r="C4" s="3">
+        <v>4.7770558499942303E-5</v>
+      </c>
+      <c r="D4" s="2">
+        <v>-4.7770558499942398E-5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>8</v>
+      </c>
+      <c r="C5" s="2">
+        <v>3.3505902313081103E-5</v>
+      </c>
+      <c r="D5" s="2">
+        <v>-3.3505902313081401E-5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>42</v>
+      </c>
+      <c r="B6">
+        <v>43</v>
+      </c>
+      <c r="C6" s="1">
+        <v>2.28997850826505E-2</v>
+      </c>
+      <c r="D6" s="1">
+        <v>-2.28997850826505E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1.06035819245887E-2</v>
+      </c>
+      <c r="D7" s="1">
+        <v>-1.06035819245887E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>48</v>
+      </c>
+      <c r="B8">
+        <v>49</v>
+      </c>
+      <c r="C8" s="1">
+        <v>9.4255399794300303E-3</v>
+      </c>
+      <c r="D8" s="1">
+        <v>-9.4255399794300199E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>52</v>
+      </c>
+      <c r="B9">
+        <v>53</v>
+      </c>
+      <c r="C9" s="1">
+        <v>7.7457540362754797E-3</v>
+      </c>
+      <c r="D9" s="1">
+        <v>-7.7457540362754797E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>35</v>
+      </c>
+      <c r="B10">
+        <v>36</v>
+      </c>
+      <c r="C10" s="1">
+        <v>6.84527512856102E-3</v>
+      </c>
+      <c r="D10" s="1">
+        <v>-6.84527512856102E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>49</v>
+      </c>
+      <c r="B11">
+        <v>50</v>
+      </c>
+      <c r="C11" s="1">
+        <v>4.7600695702273302E-3</v>
+      </c>
+      <c r="D11" s="1">
+        <v>-4.7600695702273398E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>19</v>
+      </c>
+      <c r="B12">
+        <v>20</v>
+      </c>
+      <c r="C12" s="1">
+        <v>3.87686119911045E-3</v>
+      </c>
+      <c r="D12" s="1">
+        <v>-3.8768611991105398E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>8</v>
+      </c>
+      <c r="B13">
+        <v>9</v>
+      </c>
+      <c r="C13" s="1">
+        <v>3.5889305824166901E-3</v>
+      </c>
+      <c r="D13" s="1">
+        <v>-3.5889305824166901E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1">
+        <v>3.5061717013034599E-3</v>
+      </c>
+      <c r="D14" s="1">
+        <v>-3.5061717013034699E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>40</v>
+      </c>
+      <c r="B15">
+        <v>41</v>
+      </c>
+      <c r="C15" s="1">
+        <v>2.9771747187393302E-3</v>
+      </c>
+      <c r="D15" s="1">
+        <v>-2.9771747187393302E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>39</v>
+      </c>
+      <c r="B16">
+        <v>40</v>
+      </c>
+      <c r="C16" s="1">
+        <v>2.41504259676975E-3</v>
+      </c>
+      <c r="D16" s="1">
+        <v>-2.41504259676975E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>43</v>
+      </c>
+      <c r="B17">
+        <v>44</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1.73834651483259E-3</v>
+      </c>
+      <c r="D17" s="1">
+        <v>-1.73834651483259E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>37</v>
+      </c>
+      <c r="B18">
+        <v>38</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1.4464385223429399E-3</v>
+      </c>
+      <c r="D18" s="1">
+        <v>-1.4464385223429499E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>38</v>
+      </c>
+      <c r="B19">
+        <v>39</v>
+      </c>
+      <c r="C19" s="1">
+        <v>1.3589362152040701E-3</v>
+      </c>
+      <c r="D19" s="1">
+        <v>-1.3589362152040499E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>5</v>
+      </c>
+      <c r="B20">
+        <v>6</v>
+      </c>
+      <c r="C20" s="1">
+        <v>1.0086188168671401E-3</v>
+      </c>
+      <c r="D20" s="1">
+        <v>-1.0086188168671401E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21" s="1">
+        <v>9.4617606286174496E-4</v>
+      </c>
+      <c r="D21" s="1">
+        <v>-9.4617606286174995E-4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>47</v>
+      </c>
+      <c r="B22">
+        <v>48</v>
+      </c>
+      <c r="C22" s="1">
+        <v>8.4859690089016397E-4</v>
+      </c>
+      <c r="D22" s="1">
+        <v>-8.4859690089016896E-4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>18</v>
+      </c>
+      <c r="B23">
+        <v>19</v>
+      </c>
+      <c r="C23" s="1">
+        <v>8.11768717507543E-4</v>
+      </c>
+      <c r="D23" s="1">
+        <v>-8.1176871750754105E-4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>2</v>
+      </c>
+      <c r="B24">
+        <v>3</v>
+      </c>
+      <c r="C24" s="1">
+        <v>7.0788869784729996E-4</v>
+      </c>
+      <c r="D24" s="1">
+        <v>-7.0788869784729996E-4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>22</v>
+      </c>
+      <c r="B25">
+        <v>23</v>
+      </c>
+      <c r="C25" s="1">
+        <v>6.3539583217619403E-4</v>
+      </c>
+      <c r="D25" s="1">
+        <v>-6.35395832176195E-4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>41</v>
+      </c>
+      <c r="B26">
+        <v>42</v>
+      </c>
+      <c r="C26" s="1">
+        <v>6.3234455557617997E-4</v>
+      </c>
+      <c r="D26" s="1">
+        <v>-6.3234455557617704E-4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>51</v>
+      </c>
+      <c r="B27">
+        <v>52</v>
+      </c>
+      <c r="C27" s="1">
+        <v>5.6017733500225101E-4</v>
+      </c>
+      <c r="D27" s="1">
+        <v>-5.6017733500225003E-4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>6</v>
+      </c>
+      <c r="B28">
+        <v>7</v>
+      </c>
+      <c r="C28" s="1">
+        <v>5.2378997056075403E-4</v>
+      </c>
+      <c r="D28" s="1">
+        <v>-5.2378997056075403E-4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>24</v>
+      </c>
+      <c r="B29">
+        <v>25</v>
+      </c>
+      <c r="C29" s="1">
+        <v>5.1039904780023201E-4</v>
+      </c>
+      <c r="D29" s="1">
+        <v>-5.1039904780023201E-4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>34</v>
+      </c>
+      <c r="B30">
+        <v>35</v>
+      </c>
+      <c r="C30" s="1">
+        <v>4.6453329598505899E-4</v>
+      </c>
+      <c r="D30" s="1">
+        <v>-4.6453329598505899E-4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31">
+        <v>30</v>
+      </c>
+      <c r="C31" s="1">
+        <v>4.1829812175931102E-4</v>
+      </c>
+      <c r="D31" s="1">
+        <v>-4.1829812175930999E-4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>21</v>
+      </c>
+      <c r="B32">
+        <v>22</v>
+      </c>
+      <c r="C32" s="1">
+        <v>4.0244608799829901E-4</v>
+      </c>
+      <c r="D32" s="1">
+        <v>-4.0244608799829901E-4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>16</v>
+      </c>
+      <c r="B33">
+        <v>17</v>
+      </c>
+      <c r="C33" s="1">
+        <v>3.9778805087951902E-4</v>
+      </c>
+      <c r="D33" s="1">
+        <v>-3.9778805087951799E-4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>36</v>
+      </c>
+      <c r="B34">
+        <v>37</v>
+      </c>
+      <c r="C34" s="1">
+        <v>3.9459289962526201E-4</v>
+      </c>
+      <c r="D34" s="1">
+        <v>-3.9459289962526299E-4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>14</v>
+      </c>
+      <c r="B35">
+        <v>15</v>
+      </c>
+      <c r="C35" s="1">
+        <v>3.3835713346842502E-4</v>
+      </c>
+      <c r="D35" s="1">
+        <v>-3.3835713346842301E-4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>23</v>
+      </c>
+      <c r="B36">
+        <v>24</v>
+      </c>
+      <c r="C36" s="1">
+        <v>3.0440472721977798E-4</v>
+      </c>
+      <c r="D36" s="1">
+        <v>-3.04404727219777E-4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>50</v>
+      </c>
+      <c r="B37">
+        <v>51</v>
+      </c>
+      <c r="C37" s="1">
+        <v>2.8691141177479801E-4</v>
+      </c>
+      <c r="D37" s="1">
+        <v>-2.86911411774796E-4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>44</v>
+      </c>
+      <c r="B38">
+        <v>45</v>
+      </c>
+      <c r="C38" s="1">
+        <v>2.8046114505346899E-4</v>
+      </c>
+      <c r="D38" s="1">
+        <v>-2.8046114505346899E-4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>46</v>
+      </c>
+      <c r="B39">
+        <v>47</v>
+      </c>
+      <c r="C39" s="1">
+        <v>2.7995470565579899E-4</v>
+      </c>
+      <c r="D39" s="1">
+        <v>-2.7995470565579899E-4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>13</v>
+      </c>
+      <c r="B40">
+        <v>14</v>
+      </c>
+      <c r="C40" s="1">
+        <v>2.7948793060825802E-4</v>
+      </c>
+      <c r="D40" s="1">
+        <v>-2.7948793060825802E-4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>30</v>
+      </c>
+      <c r="B41">
+        <v>31</v>
+      </c>
+      <c r="C41" s="1">
+        <v>2.5617364470363998E-4</v>
+      </c>
+      <c r="D41" s="1">
+        <v>-2.56173644703639E-4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>25</v>
+      </c>
+      <c r="B42">
+        <v>26</v>
+      </c>
+      <c r="C42" s="1">
+        <v>2.4778527616053502E-4</v>
+      </c>
+      <c r="D42" s="1">
+        <v>-2.4778527616053502E-4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>15</v>
+      </c>
+      <c r="B43">
+        <v>16</v>
+      </c>
+      <c r="C43" s="1">
+        <v>2.4398780843343999E-4</v>
+      </c>
+      <c r="D43" s="1">
+        <v>-2.4398780843343999E-4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>26</v>
+      </c>
+      <c r="B44">
+        <v>27</v>
+      </c>
+      <c r="C44" s="1">
+        <v>2.23969069728345E-4</v>
+      </c>
+      <c r="D44" s="1">
+        <v>-2.23969069728345E-4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>27</v>
+      </c>
+      <c r="B45">
+        <v>28</v>
+      </c>
+      <c r="C45" s="1">
+        <v>2.1875119446126699E-4</v>
+      </c>
+      <c r="D45" s="1">
+        <v>-2.1875119446126699E-4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>17</v>
+      </c>
+      <c r="B46">
+        <v>18</v>
+      </c>
+      <c r="C46" s="1">
+        <v>2.0267659464083201E-4</v>
+      </c>
+      <c r="D46" s="1">
+        <v>-2.0267659464083201E-4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>20</v>
+      </c>
+      <c r="B47">
+        <v>21</v>
+      </c>
+      <c r="C47" s="1">
+        <v>1.9072422816232001E-4</v>
+      </c>
+      <c r="D47" s="1">
+        <v>-1.9072422816232101E-4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>10</v>
+      </c>
+      <c r="B48">
+        <v>11</v>
+      </c>
+      <c r="C48" s="1">
+        <v>1.89842035083348E-4</v>
+      </c>
+      <c r="D48" s="1">
+        <v>-1.89842035083348E-4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>11</v>
+      </c>
+      <c r="B49">
+        <v>12</v>
+      </c>
+      <c r="C49" s="1">
+        <v>1.7997942447888599E-4</v>
+      </c>
+      <c r="D49" s="1">
+        <v>-1.7997942447888599E-4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>33</v>
+      </c>
+      <c r="B50">
+        <v>34</v>
+      </c>
+      <c r="C50" s="1">
+        <v>1.76593070049245E-4</v>
+      </c>
+      <c r="D50" s="1">
+        <v>-1.76593070049245E-4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>32</v>
+      </c>
+      <c r="B51">
+        <v>33</v>
+      </c>
+      <c r="C51" s="1">
+        <v>1.63958215062931E-4</v>
+      </c>
+      <c r="D51" s="1">
+        <v>-1.63958215062933E-4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>31</v>
+      </c>
+      <c r="B52">
+        <v>32</v>
+      </c>
+      <c r="C52" s="1">
+        <v>1.48182686944136E-4</v>
+      </c>
+      <c r="D52" s="1">
+        <v>-1.48182686944136E-4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>12</v>
+      </c>
+      <c r="B53">
+        <v>13</v>
+      </c>
+      <c r="C53" s="1">
+        <v>1.2417155237629801E-4</v>
+      </c>
+      <c r="D53" s="1">
+        <v>-1.2417155237629801E-4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>3</v>
+      </c>
+      <c r="B54">
+        <v>4</v>
+      </c>
+      <c r="C54" s="1">
+        <v>1.13253498458895E-4</v>
+      </c>
+      <c r="D54" s="1">
+        <v>-1.13253498458894E-4</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D54">
+    <sortCondition descending="1" ref="C1:C54"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D54"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="4" width="22" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>42</v>
+      </c>
+      <c r="B2">
+        <v>43</v>
+      </c>
+      <c r="C2" s="4">
+        <f>ABS(imported!C6)</f>
+        <v>2.28997850826505E-2</v>
+      </c>
+      <c r="D2" s="4">
+        <f>ABS(imported!D6)</f>
+        <v>2.28997850826505E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3" s="4">
+        <f>ABS(imported!C7)</f>
+        <v>1.06035819245887E-2</v>
+      </c>
+      <c r="D3" s="4">
+        <f>ABS(imported!D7)</f>
+        <v>1.06035819245887E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>48</v>
+      </c>
+      <c r="B4">
+        <v>49</v>
+      </c>
+      <c r="C4" s="4">
+        <f>ABS(imported!C8)</f>
+        <v>9.4255399794300303E-3</v>
+      </c>
+      <c r="D4" s="4">
+        <f>ABS(imported!D8)</f>
+        <v>9.4255399794300199E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>52</v>
+      </c>
+      <c r="B5">
+        <v>53</v>
+      </c>
+      <c r="C5" s="4">
+        <f>ABS(imported!C9)</f>
+        <v>7.7457540362754797E-3</v>
+      </c>
+      <c r="D5" s="4">
+        <f>ABS(imported!D9)</f>
+        <v>7.7457540362754797E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>35</v>
+      </c>
+      <c r="B6">
+        <v>36</v>
+      </c>
+      <c r="C6" s="4">
+        <f>ABS(imported!C10)</f>
+        <v>6.84527512856102E-3</v>
+      </c>
+      <c r="D6" s="4">
+        <f>ABS(imported!D10)</f>
+        <v>6.84527512856102E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>49</v>
+      </c>
+      <c r="B7">
+        <v>50</v>
+      </c>
+      <c r="C7" s="4">
+        <f>ABS(imported!C11)</f>
+        <v>4.7600695702273302E-3</v>
+      </c>
+      <c r="D7" s="4">
+        <f>ABS(imported!D11)</f>
+        <v>4.7600695702273398E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>19</v>
+      </c>
+      <c r="B8">
+        <v>20</v>
+      </c>
+      <c r="C8" s="4">
+        <f>ABS(imported!C12)</f>
+        <v>3.87686119911045E-3</v>
+      </c>
+      <c r="D8" s="4">
+        <f>ABS(imported!D12)</f>
+        <v>3.8768611991105398E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>9</v>
+      </c>
+      <c r="C9" s="4">
+        <f>ABS(imported!C13)</f>
+        <v>3.5889305824166901E-3</v>
+      </c>
+      <c r="D9" s="4">
+        <f>ABS(imported!D13)</f>
+        <v>3.5889305824166901E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" s="4">
+        <f>ABS(imported!C14)</f>
+        <v>3.5061717013034599E-3</v>
+      </c>
+      <c r="D10" s="4">
+        <f>ABS(imported!D14)</f>
+        <v>3.5061717013034699E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>40</v>
+      </c>
+      <c r="B11">
+        <v>41</v>
+      </c>
+      <c r="C11" s="4">
+        <f>ABS(imported!C15)</f>
+        <v>2.9771747187393302E-3</v>
+      </c>
+      <c r="D11" s="4">
+        <f>ABS(imported!D15)</f>
+        <v>2.9771747187393302E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>39</v>
+      </c>
+      <c r="B12">
+        <v>40</v>
+      </c>
+      <c r="C12" s="4">
+        <f>ABS(imported!C16)</f>
+        <v>2.41504259676975E-3</v>
+      </c>
+      <c r="D12" s="4">
+        <f>ABS(imported!D16)</f>
+        <v>2.41504259676975E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>43</v>
+      </c>
+      <c r="B13">
+        <v>44</v>
+      </c>
+      <c r="C13" s="4">
+        <f>ABS(imported!C17)</f>
+        <v>1.73834651483259E-3</v>
+      </c>
+      <c r="D13" s="4">
+        <f>ABS(imported!D17)</f>
+        <v>1.73834651483259E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>37</v>
+      </c>
+      <c r="B14">
+        <v>38</v>
+      </c>
+      <c r="C14" s="4">
+        <f>ABS(imported!C18)</f>
+        <v>1.4464385223429399E-3</v>
+      </c>
+      <c r="D14" s="4">
+        <f>ABS(imported!D18)</f>
+        <v>1.4464385223429499E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>38</v>
+      </c>
+      <c r="B15">
+        <v>39</v>
+      </c>
+      <c r="C15" s="4">
+        <f>ABS(imported!C19)</f>
+        <v>1.3589362152040701E-3</v>
+      </c>
+      <c r="D15" s="4">
+        <f>ABS(imported!D19)</f>
+        <v>1.3589362152040499E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>5</v>
+      </c>
+      <c r="B16">
+        <v>6</v>
+      </c>
+      <c r="C16" s="4">
+        <f>ABS(imported!C20)</f>
+        <v>1.0086188168671401E-3</v>
+      </c>
+      <c r="D16" s="4">
+        <f>ABS(imported!D20)</f>
+        <v>1.0086188168671401E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17" s="4">
+        <f>ABS(imported!C21)</f>
+        <v>9.4617606286174496E-4</v>
+      </c>
+      <c r="D17" s="4">
+        <f>ABS(imported!D21)</f>
+        <v>9.4617606286174995E-4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>47</v>
+      </c>
+      <c r="B18">
+        <v>48</v>
+      </c>
+      <c r="C18" s="4">
+        <f>ABS(imported!C22)</f>
+        <v>8.4859690089016397E-4</v>
+      </c>
+      <c r="D18" s="4">
+        <f>ABS(imported!D22)</f>
+        <v>8.4859690089016896E-4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>19</v>
+      </c>
+      <c r="C19" s="4">
+        <f>ABS(imported!C23)</f>
+        <v>8.11768717507543E-4</v>
+      </c>
+      <c r="D19" s="4">
+        <f>ABS(imported!D23)</f>
+        <v>8.1176871750754105E-4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>2</v>
+      </c>
+      <c r="B20">
+        <v>3</v>
+      </c>
+      <c r="C20" s="4">
+        <f>ABS(imported!C24)</f>
+        <v>7.0788869784729996E-4</v>
+      </c>
+      <c r="D20" s="4">
+        <f>ABS(imported!D24)</f>
+        <v>7.0788869784729996E-4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>22</v>
+      </c>
+      <c r="B21">
+        <v>23</v>
+      </c>
+      <c r="C21" s="4">
+        <f>ABS(imported!C25)</f>
+        <v>6.3539583217619403E-4</v>
+      </c>
+      <c r="D21" s="4">
+        <f>ABS(imported!D25)</f>
+        <v>6.35395832176195E-4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>41</v>
+      </c>
+      <c r="B22">
+        <v>42</v>
+      </c>
+      <c r="C22" s="4">
+        <f>ABS(imported!C26)</f>
+        <v>6.3234455557617997E-4</v>
+      </c>
+      <c r="D22" s="4">
+        <f>ABS(imported!D26)</f>
+        <v>6.3234455557617704E-4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>51</v>
+      </c>
+      <c r="B23">
+        <v>52</v>
+      </c>
+      <c r="C23" s="4">
+        <f>ABS(imported!C27)</f>
+        <v>5.6017733500225101E-4</v>
+      </c>
+      <c r="D23" s="4">
+        <f>ABS(imported!D27)</f>
+        <v>5.6017733500225003E-4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>6</v>
+      </c>
+      <c r="B24">
+        <v>7</v>
+      </c>
+      <c r="C24" s="4">
+        <f>ABS(imported!C28)</f>
+        <v>5.2378997056075403E-4</v>
+      </c>
+      <c r="D24" s="4">
+        <f>ABS(imported!D28)</f>
+        <v>5.2378997056075403E-4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>25</v>
+      </c>
+      <c r="C25" s="4">
+        <f>ABS(imported!C29)</f>
+        <v>5.1039904780023201E-4</v>
+      </c>
+      <c r="D25" s="4">
+        <f>ABS(imported!D29)</f>
+        <v>5.1039904780023201E-4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>34</v>
+      </c>
+      <c r="B26">
+        <v>35</v>
+      </c>
+      <c r="C26" s="4">
+        <f>ABS(imported!C30)</f>
+        <v>4.6453329598505899E-4</v>
+      </c>
+      <c r="D26" s="4">
+        <f>ABS(imported!D30)</f>
+        <v>4.6453329598505899E-4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>29</v>
+      </c>
+      <c r="B27">
+        <v>30</v>
+      </c>
+      <c r="C27" s="4">
+        <f>ABS(imported!C31)</f>
+        <v>4.1829812175931102E-4</v>
+      </c>
+      <c r="D27" s="4">
+        <f>ABS(imported!D31)</f>
+        <v>4.1829812175930999E-4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>21</v>
+      </c>
+      <c r="B28">
+        <v>22</v>
+      </c>
+      <c r="C28" s="4">
+        <f>ABS(imported!C32)</f>
+        <v>4.0244608799829901E-4</v>
+      </c>
+      <c r="D28" s="4">
+        <f>ABS(imported!D32)</f>
+        <v>4.0244608799829901E-4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>16</v>
+      </c>
+      <c r="B29">
+        <v>17</v>
+      </c>
+      <c r="C29" s="4">
+        <f>ABS(imported!C33)</f>
+        <v>3.9778805087951902E-4</v>
+      </c>
+      <c r="D29" s="4">
+        <f>ABS(imported!D33)</f>
+        <v>3.9778805087951799E-4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>36</v>
+      </c>
+      <c r="B30">
+        <v>37</v>
+      </c>
+      <c r="C30" s="4">
+        <f>ABS(imported!C34)</f>
+        <v>3.9459289962526201E-4</v>
+      </c>
+      <c r="D30" s="4">
+        <f>ABS(imported!D34)</f>
+        <v>3.9459289962526299E-4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>14</v>
+      </c>
+      <c r="B31">
+        <v>15</v>
+      </c>
+      <c r="C31" s="4">
+        <f>ABS(imported!C35)</f>
+        <v>3.3835713346842502E-4</v>
+      </c>
+      <c r="D31" s="4">
+        <f>ABS(imported!D35)</f>
+        <v>3.3835713346842301E-4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>23</v>
+      </c>
+      <c r="B32">
+        <v>24</v>
+      </c>
+      <c r="C32" s="4">
+        <f>ABS(imported!C36)</f>
+        <v>3.0440472721977798E-4</v>
+      </c>
+      <c r="D32" s="4">
+        <f>ABS(imported!D36)</f>
+        <v>3.04404727219777E-4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>50</v>
+      </c>
+      <c r="B33">
+        <v>51</v>
+      </c>
+      <c r="C33" s="4">
+        <f>ABS(imported!C37)</f>
+        <v>2.8691141177479801E-4</v>
+      </c>
+      <c r="D33" s="4">
+        <f>ABS(imported!D37)</f>
+        <v>2.86911411774796E-4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>44</v>
+      </c>
+      <c r="B34">
+        <v>45</v>
+      </c>
+      <c r="C34" s="4">
+        <f>ABS(imported!C38)</f>
+        <v>2.8046114505346899E-4</v>
+      </c>
+      <c r="D34" s="4">
+        <f>ABS(imported!D38)</f>
+        <v>2.8046114505346899E-4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>46</v>
+      </c>
+      <c r="B35">
+        <v>47</v>
+      </c>
+      <c r="C35" s="4">
+        <f>ABS(imported!C39)</f>
+        <v>2.7995470565579899E-4</v>
+      </c>
+      <c r="D35" s="4">
+        <f>ABS(imported!D39)</f>
+        <v>2.7995470565579899E-4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>13</v>
+      </c>
+      <c r="B36">
+        <v>14</v>
+      </c>
+      <c r="C36" s="4">
+        <f>ABS(imported!C40)</f>
+        <v>2.7948793060825802E-4</v>
+      </c>
+      <c r="D36" s="4">
+        <f>ABS(imported!D40)</f>
+        <v>2.7948793060825802E-4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>30</v>
+      </c>
+      <c r="B37">
+        <v>31</v>
+      </c>
+      <c r="C37" s="4">
+        <f>ABS(imported!C41)</f>
+        <v>2.5617364470363998E-4</v>
+      </c>
+      <c r="D37" s="4">
+        <f>ABS(imported!D41)</f>
+        <v>2.56173644703639E-4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>25</v>
+      </c>
+      <c r="B38">
+        <v>26</v>
+      </c>
+      <c r="C38" s="4">
+        <f>ABS(imported!C42)</f>
+        <v>2.4778527616053502E-4</v>
+      </c>
+      <c r="D38" s="4">
+        <f>ABS(imported!D42)</f>
+        <v>2.4778527616053502E-4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>15</v>
+      </c>
+      <c r="B39">
+        <v>16</v>
+      </c>
+      <c r="C39" s="4">
+        <f>ABS(imported!C43)</f>
+        <v>2.4398780843343999E-4</v>
+      </c>
+      <c r="D39" s="4">
+        <f>ABS(imported!D43)</f>
+        <v>2.4398780843343999E-4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>26</v>
+      </c>
+      <c r="B40">
+        <v>27</v>
+      </c>
+      <c r="C40" s="4">
+        <f>ABS(imported!C44)</f>
+        <v>2.23969069728345E-4</v>
+      </c>
+      <c r="D40" s="4">
+        <f>ABS(imported!D44)</f>
+        <v>2.23969069728345E-4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>27</v>
+      </c>
+      <c r="B41">
+        <v>28</v>
+      </c>
+      <c r="C41" s="4">
+        <f>ABS(imported!C45)</f>
+        <v>2.1875119446126699E-4</v>
+      </c>
+      <c r="D41" s="4">
+        <f>ABS(imported!D45)</f>
+        <v>2.1875119446126699E-4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>17</v>
+      </c>
+      <c r="B42">
+        <v>18</v>
+      </c>
+      <c r="C42" s="4">
+        <f>ABS(imported!C46)</f>
+        <v>2.0267659464083201E-4</v>
+      </c>
+      <c r="D42" s="4">
+        <f>ABS(imported!D46)</f>
+        <v>2.0267659464083201E-4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>20</v>
+      </c>
+      <c r="B43">
+        <v>21</v>
+      </c>
+      <c r="C43" s="4">
+        <f>ABS(imported!C47)</f>
+        <v>1.9072422816232001E-4</v>
+      </c>
+      <c r="D43" s="4">
+        <f>ABS(imported!D47)</f>
+        <v>1.9072422816232101E-4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>10</v>
+      </c>
+      <c r="B44">
+        <v>11</v>
+      </c>
+      <c r="C44" s="4">
+        <f>ABS(imported!C48)</f>
+        <v>1.89842035083348E-4</v>
+      </c>
+      <c r="D44" s="4">
+        <f>ABS(imported!D48)</f>
+        <v>1.89842035083348E-4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>11</v>
+      </c>
+      <c r="B45">
+        <v>12</v>
+      </c>
+      <c r="C45" s="4">
+        <f>ABS(imported!C49)</f>
+        <v>1.7997942447888599E-4</v>
+      </c>
+      <c r="D45" s="4">
+        <f>ABS(imported!D49)</f>
+        <v>1.7997942447888599E-4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>33</v>
+      </c>
+      <c r="B46">
+        <v>34</v>
+      </c>
+      <c r="C46" s="4">
+        <f>ABS(imported!C50)</f>
+        <v>1.76593070049245E-4</v>
+      </c>
+      <c r="D46" s="4">
+        <f>ABS(imported!D50)</f>
+        <v>1.76593070049245E-4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>32</v>
+      </c>
+      <c r="B47">
+        <v>33</v>
+      </c>
+      <c r="C47" s="4">
+        <f>ABS(imported!C51)</f>
+        <v>1.63958215062931E-4</v>
+      </c>
+      <c r="D47" s="4">
+        <f>ABS(imported!D51)</f>
+        <v>1.63958215062933E-4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>31</v>
+      </c>
+      <c r="B48">
+        <v>32</v>
+      </c>
+      <c r="C48" s="4">
+        <f>ABS(imported!C52)</f>
+        <v>1.48182686944136E-4</v>
+      </c>
+      <c r="D48" s="4">
+        <f>ABS(imported!D52)</f>
+        <v>1.48182686944136E-4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>12</v>
+      </c>
+      <c r="B49">
+        <v>13</v>
+      </c>
+      <c r="C49" s="4">
+        <f>ABS(imported!C53)</f>
+        <v>1.2417155237629801E-4</v>
+      </c>
+      <c r="D49" s="4">
+        <f>ABS(imported!D53)</f>
+        <v>1.2417155237629801E-4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>3</v>
+      </c>
+      <c r="B50">
+        <v>4</v>
+      </c>
+      <c r="C50" s="4">
+        <f>ABS(imported!C54)</f>
+        <v>1.13253498458895E-4</v>
+      </c>
+      <c r="D50" s="4">
+        <f>ABS(imported!D54)</f>
+        <v>1.13253498458894E-4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>45</v>
+      </c>
+      <c r="B51">
+        <v>46</v>
+      </c>
+      <c r="C51" s="4">
+        <f>ABS(imported!C2)</f>
+        <v>7.5521497601685304E-5</v>
+      </c>
+      <c r="D51" s="4">
+        <f>ABS(imported!D2)</f>
+        <v>7.5521497601685399E-5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>28</v>
+      </c>
+      <c r="B52">
+        <v>29</v>
+      </c>
+      <c r="C52" s="4">
+        <f>ABS(imported!C3)</f>
+        <v>6.5715416017797106E-5</v>
+      </c>
+      <c r="D52" s="4">
+        <f>ABS(imported!D3)</f>
+        <v>6.5715416017797106E-5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>9</v>
+      </c>
+      <c r="B53">
+        <v>10</v>
+      </c>
+      <c r="C53" s="4">
+        <f>ABS(imported!C4)</f>
+        <v>4.7770558499942303E-5</v>
+      </c>
+      <c r="D53" s="4">
+        <f>ABS(imported!D4)</f>
+        <v>4.7770558499942398E-5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>7</v>
+      </c>
+      <c r="B54">
+        <v>8</v>
+      </c>
+      <c r="C54" s="4">
+        <f>ABS(imported!C5)</f>
+        <v>3.3505902313081103E-5</v>
+      </c>
+      <c r="D54" s="4">
+        <f>ABS(imported!D5)</f>
+        <v>3.3505902313081401E-5</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:D1">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D54">
+      <sortCondition descending="1" ref="C1:C54"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>